<commit_message>
Work on CoolProp and Cantera Comparison
</commit_message>
<xml_diff>
--- a/TheEngine/Regen Solver/canterafiles/exhaustgastandk.xlsx
+++ b/TheEngine/Regen Solver/canterafiles/exhaustgastandk.xlsx
@@ -417,13 +417,13 @@
         <v>0.2</v>
       </c>
       <c r="C2">
-        <v>627.3345163610192</v>
+        <v>627.3345163610151</v>
       </c>
       <c r="D2">
-        <v>1.144286610547475</v>
+        <v>1.144286610547476</v>
       </c>
       <c r="E2">
-        <v>1.144286610547475</v>
+        <v>1.144286610547476</v>
       </c>
       <c r="F2">
         <v>24.27961346789373</v>
@@ -437,7 +437,7 @@
         <v>0.4</v>
       </c>
       <c r="C3">
-        <v>804.993971045369</v>
+        <v>804.9939710453643</v>
       </c>
       <c r="D3">
         <v>1.162412336150831</v>
@@ -457,13 +457,13 @@
         <v>0.6000000000000001</v>
       </c>
       <c r="C4">
-        <v>1022.623307266333</v>
+        <v>1022.623307266323</v>
       </c>
       <c r="D4">
-        <v>1.159392044626535</v>
+        <v>1.159392044626536</v>
       </c>
       <c r="E4">
-        <v>1.159392044626535</v>
+        <v>1.159392044626536</v>
       </c>
       <c r="F4">
         <v>20.63549585329684</v>
@@ -477,13 +477,13 @@
         <v>0.8</v>
       </c>
       <c r="C5">
-        <v>1136.538183357494</v>
+        <v>1136.538183357485</v>
       </c>
       <c r="D5">
-        <v>1.169257307985683</v>
+        <v>1.169257307985684</v>
       </c>
       <c r="E5">
-        <v>1.169257307985683</v>
+        <v>1.169257307985684</v>
       </c>
       <c r="F5">
         <v>20.0849221870714</v>
@@ -497,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1190.672067971682</v>
+        <v>1190.672067971679</v>
       </c>
       <c r="D6">
         <v>1.185186252329243</v>
@@ -517,13 +517,13 @@
         <v>1.2</v>
       </c>
       <c r="C7">
-        <v>1226.20814185898</v>
+        <v>1226.208141858112</v>
       </c>
       <c r="D7">
-        <v>1.202174299453108</v>
+        <v>1.202174299453168</v>
       </c>
       <c r="E7">
-        <v>1.202174299453108</v>
+        <v>1.202174299453168</v>
       </c>
       <c r="F7">
         <v>18.91980442792249</v>
@@ -537,13 +537,13 @@
         <v>1.4</v>
       </c>
       <c r="C8">
-        <v>1254.124533811811</v>
+        <v>1254.124533811699</v>
       </c>
       <c r="D8">
-        <v>1.219064952622682</v>
+        <v>1.21906495262269</v>
       </c>
       <c r="E8">
-        <v>1.219064952622682</v>
+        <v>1.21906495262269</v>
       </c>
       <c r="F8">
         <v>18.47825271937595</v>
@@ -557,7 +557,7 @@
         <v>1.6</v>
       </c>
       <c r="C9">
-        <v>1278.027345227458</v>
+        <v>1278.027345227459</v>
       </c>
       <c r="D9">
         <v>1.23554797727587</v>
@@ -577,7 +577,7 @@
         <v>1.8</v>
       </c>
       <c r="C10">
-        <v>1299.630066444856</v>
+        <v>1299.630066444858</v>
       </c>
       <c r="D10">
         <v>1.251508683326736</v>
@@ -597,13 +597,13 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>1320.045561109063</v>
+        <v>1320.045561108795</v>
       </c>
       <c r="D11">
-        <v>1.266882910997247</v>
+        <v>1.266882910997263</v>
       </c>
       <c r="E11">
-        <v>1.266882910997247</v>
+        <v>1.266882910997263</v>
       </c>
       <c r="F11">
         <v>17.56874969562816</v>
@@ -617,13 +617,13 @@
         <v>2.2</v>
       </c>
       <c r="C12">
-        <v>1340.211740034509</v>
+        <v>1340.211740032537</v>
       </c>
       <c r="D12">
-        <v>1.281611021363786</v>
+        <v>1.281611021363901</v>
       </c>
       <c r="E12">
-        <v>1.281611021363786</v>
+        <v>1.281611021363901</v>
       </c>
       <c r="F12">
         <v>17.36268416068665</v>
@@ -637,13 +637,13 @@
         <v>2.4</v>
       </c>
       <c r="C13">
-        <v>1361.138568749618</v>
+        <v>1361.138568749649</v>
       </c>
       <c r="D13">
-        <v>1.295608202316385</v>
+        <v>1.295608202316383</v>
       </c>
       <c r="E13">
-        <v>1.295608202316385</v>
+        <v>1.295608202316383</v>
       </c>
       <c r="F13">
         <v>17.19336034733466</v>
@@ -657,13 +657,13 @@
         <v>2.6</v>
       </c>
       <c r="C14">
-        <v>1384.276585507177</v>
+        <v>1384.27658550724</v>
       </c>
       <c r="D14">
-        <v>1.308706284303772</v>
+        <v>1.308706284303769</v>
       </c>
       <c r="E14">
-        <v>1.308706284303772</v>
+        <v>1.308706284303769</v>
       </c>
       <c r="F14">
         <v>17.05921669698788</v>
@@ -677,13 +677,13 @@
         <v>2.8</v>
       </c>
       <c r="C15">
-        <v>1413.256502365632</v>
+        <v>1413.256502365753</v>
       </c>
       <c r="D15">
-        <v>1.320319621878529</v>
+        <v>1.320319621878523</v>
       </c>
       <c r="E15">
-        <v>1.320319621878529</v>
+        <v>1.320319621878523</v>
       </c>
       <c r="F15">
         <v>16.97094692585523</v>
@@ -697,13 +697,13 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>1480.718438732077</v>
+        <v>1480.71843873223</v>
       </c>
       <c r="D16">
-        <v>1.323921444718629</v>
+        <v>1.323921444718622</v>
       </c>
       <c r="E16">
-        <v>1.323921444718629</v>
+        <v>1.323921444718622</v>
       </c>
       <c r="F16">
         <v>17.10386391964836</v>
@@ -717,13 +717,13 @@
         <v>3.2</v>
       </c>
       <c r="C17">
-        <v>1604.938919816689</v>
+        <v>1604.938919816793</v>
       </c>
       <c r="D17">
-        <v>1.315519368163474</v>
+        <v>1.31551936816347</v>
       </c>
       <c r="E17">
-        <v>1.315519368163474</v>
+        <v>1.31551936816347</v>
       </c>
       <c r="F17">
         <v>17.58024074011909</v>
@@ -737,13 +737,13 @@
         <v>3.4</v>
       </c>
       <c r="C18">
-        <v>1725.940005994302</v>
+        <v>1725.94000599435</v>
       </c>
       <c r="D18">
-        <v>1.307227165592343</v>
+        <v>1.307227165592341</v>
       </c>
       <c r="E18">
-        <v>1.307227165592343</v>
+        <v>1.307227165592341</v>
       </c>
       <c r="F18">
         <v>18.06898071186098</v>
@@ -757,13 +757,13 @@
         <v>3.6</v>
       </c>
       <c r="C19">
-        <v>1839.348477511145</v>
+        <v>1839.348477511174</v>
       </c>
       <c r="D19">
-        <v>1.299882461534611</v>
+        <v>1.29988246153461</v>
       </c>
       <c r="E19">
-        <v>1.299882461534611</v>
+        <v>1.29988246153461</v>
       </c>
       <c r="F19">
         <v>18.54122603434792</v>
@@ -777,13 +777,13 @@
         <v>3.8</v>
       </c>
       <c r="C20">
-        <v>1945.375948809993</v>
+        <v>1945.375948810009</v>
       </c>
       <c r="D20">
-        <v>1.293389132863437</v>
+        <v>1.293389132863436</v>
       </c>
       <c r="E20">
-        <v>1.293389132863437</v>
+        <v>1.293389132863436</v>
       </c>
       <c r="F20">
         <v>18.9954356657317</v>
@@ -797,13 +797,13 @@
         <v>4</v>
       </c>
       <c r="C21">
-        <v>2044.385719778635</v>
+        <v>2044.385719778646</v>
       </c>
       <c r="D21">
-        <v>1.287629769570439</v>
+        <v>1.287629769570438</v>
       </c>
       <c r="E21">
-        <v>1.287629769570439</v>
+        <v>1.287629769570438</v>
       </c>
       <c r="F21">
         <v>19.43166183935261</v>
@@ -817,13 +817,13 @@
         <v>4.2</v>
       </c>
       <c r="C22">
-        <v>2136.713229906698</v>
+        <v>2136.713229903033</v>
       </c>
       <c r="D22">
-        <v>1.282504012404901</v>
+        <v>1.282504012404988</v>
       </c>
       <c r="E22">
-        <v>1.282504012404901</v>
+        <v>1.282504012404988</v>
       </c>
       <c r="F22">
         <v>19.85017334435259</v>
@@ -837,13 +837,13 @@
         <v>4.4</v>
       </c>
       <c r="C23">
-        <v>2222.668404801874</v>
+        <v>2222.66840479957</v>
       </c>
       <c r="D23">
-        <v>1.277928113299666</v>
+        <v>1.277928113299717</v>
       </c>
       <c r="E23">
-        <v>1.277928113299666</v>
+        <v>1.277928113299717</v>
       </c>
       <c r="F23">
         <v>20.25130588158043</v>
@@ -857,13 +857,13 @@
         <v>4.600000000000001</v>
       </c>
       <c r="C24">
-        <v>2302.543496106618</v>
+        <v>2302.543496105181</v>
       </c>
       <c r="D24">
-        <v>1.273832015569606</v>
+        <v>1.273832015569634</v>
       </c>
       <c r="E24">
-        <v>1.273832015569606</v>
+        <v>1.273832015569634</v>
       </c>
       <c r="F24">
         <v>20.63544149801777</v>
@@ -877,13 +877,13 @@
         <v>4.800000000000001</v>
       </c>
       <c r="C25">
-        <v>2376.613140548498</v>
+        <v>2376.613140547611</v>
       </c>
       <c r="D25">
-        <v>1.270156995938795</v>
+        <v>1.270156995938811</v>
       </c>
       <c r="E25">
-        <v>1.270156995938795</v>
+        <v>1.270156995938811</v>
       </c>
       <c r="F25">
         <v>21.002996829969</v>
@@ -897,13 +897,13 @@
         <v>5</v>
       </c>
       <c r="C26">
-        <v>2445.129042796305</v>
+        <v>2445.129042795768</v>
       </c>
       <c r="D26">
-        <v>1.266853929754981</v>
+        <v>1.266853929754991</v>
       </c>
       <c r="E26">
-        <v>1.266853929754981</v>
+        <v>1.266853929754991</v>
       </c>
       <c r="F26">
         <v>21.35440459271673</v>
@@ -917,13 +917,13 @@
         <v>5.2</v>
       </c>
       <c r="C27">
-        <v>2508.31336088535</v>
+        <v>2508.313360885024</v>
       </c>
       <c r="D27">
-        <v>1.263881949956176</v>
+        <v>1.263881949956182</v>
       </c>
       <c r="E27">
-        <v>1.263881949956176</v>
+        <v>1.263881949956182</v>
       </c>
       <c r="F27">
         <v>21.69009066997815</v>
@@ -937,13 +937,13 @@
         <v>5.4</v>
       </c>
       <c r="C28">
-        <v>2566.354296856139</v>
+        <v>2566.35429685595</v>
       </c>
       <c r="D28">
-        <v>1.261207307196571</v>
+        <v>1.261207307196574</v>
       </c>
       <c r="E28">
-        <v>1.261207307196571</v>
+        <v>1.261207307196574</v>
       </c>
       <c r="F28">
         <v>22.0104525060207</v>
@@ -957,13 +957,13 @@
         <v>5.600000000000001</v>
       </c>
       <c r="C29">
-        <v>2619.406388052096</v>
+        <v>2619.406388051981</v>
       </c>
       <c r="D29">
-        <v>1.258802301713912</v>
+        <v>1.258802301713914</v>
       </c>
       <c r="E29">
-        <v>1.258802301713912</v>
+        <v>1.258802301713914</v>
       </c>
       <c r="F29">
         <v>22.31584434892106</v>
@@ -977,13 +977,13 @@
         <v>5.800000000000001</v>
       </c>
       <c r="C30">
-        <v>2667.596887193128</v>
+        <v>2667.596887193078</v>
       </c>
       <c r="D30">
-        <v>1.25664420907168</v>
+        <v>1.256644209071681</v>
       </c>
       <c r="E30">
-        <v>1.25664420907168</v>
+        <v>1.256644209071681</v>
       </c>
       <c r="F30">
         <v>22.60657364604899</v>
@@ -997,13 +997,13 @@
         <v>6</v>
       </c>
       <c r="C31">
-        <v>2711.038325256477</v>
+        <v>2711.038325256431</v>
       </c>
       <c r="D31">
-        <v>1.254714168097157</v>
+        <v>1.254714168097158</v>
       </c>
       <c r="E31">
-        <v>1.254714168097157</v>
+        <v>1.254714168097158</v>
       </c>
       <c r="F31">
         <v>22.88291094235446</v>
@@ -1017,13 +1017,13 @@
         <v>6.2</v>
       </c>
       <c r="C32">
-        <v>2749.845765597487</v>
+        <v>2749.84576559746</v>
       </c>
       <c r="D32">
-        <v>1.25299604979545</v>
+        <v>1.252996049795451</v>
       </c>
       <c r="E32">
-        <v>1.25299604979545</v>
+        <v>1.252996049795451</v>
       </c>
       <c r="F32">
         <v>23.14511281974134</v>
@@ -1037,7 +1037,7 @@
         <v>6.4</v>
       </c>
       <c r="C33">
-        <v>2784.155595699476</v>
+        <v>2784.155595699465</v>
       </c>
       <c r="D33">
         <v>1.251475378974756</v>
@@ -1057,7 +1057,7 @@
         <v>6.600000000000001</v>
       </c>
       <c r="C34">
-        <v>2814.141576484812</v>
+        <v>2814.141576484809</v>
       </c>
       <c r="D34">
         <v>1.25013841865468</v>
@@ -1077,7 +1077,7 @@
         <v>6.800000000000001</v>
       </c>
       <c r="C35">
-        <v>2840.024095615203</v>
+        <v>2840.024095615206</v>
       </c>
       <c r="D35">
         <v>1.248971527201295</v>
@@ -1097,7 +1097,7 @@
         <v>7</v>
       </c>
       <c r="C36">
-        <v>2862.070347518557</v>
+        <v>2862.070347518552</v>
       </c>
       <c r="D36">
         <v>1.24796084908219</v>
@@ -1117,7 +1117,7 @@
         <v>7.2</v>
       </c>
       <c r="C37">
-        <v>2880.585915430546</v>
+        <v>2880.585915430543</v>
       </c>
       <c r="D37">
         <v>1.247092321421995</v>
@@ -1137,7 +1137,7 @@
         <v>7.4</v>
       </c>
       <c r="C38">
-        <v>2895.900562516763</v>
+        <v>2895.900562516761</v>
       </c>
       <c r="D38">
         <v>1.246351906346546</v>
@@ -1157,7 +1157,7 @@
         <v>7.600000000000001</v>
       </c>
       <c r="C39">
-        <v>2908.352067975056</v>
+        <v>2908.35206797506</v>
       </c>
       <c r="D39">
         <v>1.245725927305428</v>
@@ -1177,7 +1177,7 @@
         <v>7.800000000000001</v>
       </c>
       <c r="C40">
-        <v>2918.271453526069</v>
+        <v>2918.271453526059</v>
       </c>
       <c r="D40">
         <v>1.245201400226029</v>
@@ -1197,7 +1197,7 @@
         <v>8</v>
       </c>
       <c r="C41">
-        <v>2925.971614245647</v>
+        <v>2925.971614245654</v>
       </c>
       <c r="D41">
         <v>1.244766289705246</v>
@@ -1217,7 +1217,7 @@
         <v>8.200000000000001</v>
       </c>
       <c r="C42">
-        <v>2931.73998210332</v>
+        <v>2931.739982103316</v>
       </c>
       <c r="D42">
         <v>1.244409664207809</v>
@@ -1237,7 +1237,7 @@
         <v>8.4</v>
       </c>
       <c r="C43">
-        <v>2935.834859898261</v>
+        <v>2935.834859898251</v>
       </c>
       <c r="D43">
         <v>1.244121754720431</v>
@@ -1257,7 +1257,7 @@
         <v>8.6</v>
       </c>
       <c r="C44">
-        <v>2938.484585201969</v>
+        <v>2938.484585201979</v>
       </c>
       <c r="D44">
         <v>1.243893938323121</v>
@@ -1277,7 +1277,7 @@
         <v>8.800000000000001</v>
       </c>
       <c r="C45">
-        <v>2939.88861519744</v>
+        <v>2939.888615197439</v>
       </c>
       <c r="D45">
         <v>1.243718671229137</v>
@@ -1297,7 +1297,7 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>2940.219734213976</v>
+        <v>2940.219734213978</v>
       </c>
       <c r="D46">
         <v>1.243589393534553</v>
@@ -1317,7 +1317,7 @@
         <v>9.200000000000001</v>
       </c>
       <c r="C47">
-        <v>2939.626801069948</v>
+        <v>2939.626801069875</v>
       </c>
       <c r="D47">
         <v>1.243500421947441</v>
@@ -1337,7 +1337,7 @@
         <v>9.4</v>
       </c>
       <c r="C48">
-        <v>2938.23763836416</v>
+        <v>2938.237638364087</v>
       </c>
       <c r="D48">
         <v>1.243446841877017</v>
@@ -1357,13 +1357,13 @@
         <v>9.600000000000001</v>
       </c>
       <c r="C49">
-        <v>2936.161825935224</v>
+        <v>2936.161825935172</v>
       </c>
       <c r="D49">
-        <v>1.243424405568446</v>
+        <v>1.243424405568447</v>
       </c>
       <c r="E49">
-        <v>1.243424405568446</v>
+        <v>1.243424405568447</v>
       </c>
       <c r="F49">
         <v>25.92247600633499</v>
@@ -1377,7 +1377,7 @@
         <v>9.800000000000001</v>
       </c>
       <c r="C50">
-        <v>2933.493269687319</v>
+        <v>2933.493269687245</v>
       </c>
       <c r="D50">
         <v>1.243429439280543</v>
@@ -1397,13 +1397,13 @@
         <v>10</v>
       </c>
       <c r="C51">
-        <v>2930.312487311982</v>
+        <v>2930.312487311913</v>
       </c>
       <c r="D51">
-        <v>1.24345876123616</v>
+        <v>1.243458761236161</v>
       </c>
       <c r="E51">
-        <v>1.24345876123616</v>
+        <v>1.243458761236161</v>
       </c>
       <c r="F51">
         <v>26.11402580781791</v>
@@ -1417,7 +1417,7 @@
         <v>10.2</v>
       </c>
       <c r="C52">
-        <v>2926.688607776288</v>
+        <v>2926.688607776293</v>
       </c>
       <c r="D52">
         <v>1.243509610331704</v>
@@ -1437,7 +1437,7 @@
         <v>10.4</v>
       </c>
       <c r="C53">
-        <v>2922.681084180478</v>
+        <v>2922.681084180479</v>
       </c>
       <c r="D53">
         <v>1.243579584589183</v>
@@ -1457,7 +1457,7 @@
         <v>10.6</v>
       </c>
       <c r="C54">
-        <v>2918.341156195906</v>
+        <v>2918.341156195908</v>
       </c>
       <c r="D54">
         <v>1.243666588884117</v>
@@ -1497,7 +1497,7 @@
         <v>11</v>
       </c>
       <c r="C56">
-        <v>2908.835228751635</v>
+        <v>2908.835228751639</v>
       </c>
       <c r="D56">
         <v>1.243884580657529</v>
@@ -1517,7 +1517,7 @@
         <v>11.2</v>
       </c>
       <c r="C57">
-        <v>2903.740860193985</v>
+        <v>2903.740860193986</v>
       </c>
       <c r="D57">
         <v>1.244012544375053</v>
@@ -1537,7 +1537,7 @@
         <v>11.4</v>
       </c>
       <c r="C58">
-        <v>2898.458971726242</v>
+        <v>2898.458971726236</v>
       </c>
       <c r="D58">
         <v>1.244151431732579</v>
@@ -1557,7 +1557,7 @@
         <v>11.6</v>
       </c>
       <c r="C59">
-        <v>2893.014868426358</v>
+        <v>2893.014868426356</v>
       </c>
       <c r="D59">
         <v>1.244300135890293</v>
@@ -1577,7 +1577,7 @@
         <v>11.8</v>
       </c>
       <c r="C60">
-        <v>2887.43069887241</v>
+        <v>2887.430698872409</v>
       </c>
       <c r="D60">
         <v>1.244457673600361</v>
@@ -1597,7 +1597,7 @@
         <v>12</v>
       </c>
       <c r="C61">
-        <v>2881.725901533137</v>
+        <v>2881.72590153315</v>
       </c>
       <c r="D61">
         <v>1.244623168790929</v>
@@ -1617,7 +1617,7 @@
         <v>12.2</v>
       </c>
       <c r="C62">
-        <v>2875.917578282212</v>
+        <v>2875.917578282211</v>
       </c>
       <c r="D62">
         <v>1.244795838616336</v>
@@ -1637,7 +1637,7 @@
         <v>12.4</v>
       </c>
       <c r="C63">
-        <v>2870.020814279398</v>
+        <v>2870.020814279387</v>
       </c>
       <c r="D63">
         <v>1.244974981435063</v>
@@ -1657,7 +1657,7 @@
         <v>12.6</v>
       </c>
       <c r="C64">
-        <v>2864.048946795343</v>
+        <v>2864.048946795339</v>
       </c>
       <c r="D64">
         <v>1.245159966753183</v>
@@ -1677,7 +1677,7 @@
         <v>12.8</v>
       </c>
       <c r="C65">
-        <v>2858.013795828728</v>
+        <v>2858.013795828737</v>
       </c>
       <c r="D65">
         <v>1.245350226419826</v>
@@ -1697,7 +1697,7 @@
         <v>13</v>
       </c>
       <c r="C66">
-        <v>2851.925860051684</v>
+        <v>2851.925860051691</v>
       </c>
       <c r="D66">
         <v>1.245545247141556</v>

</xml_diff>